<commit_message>
Update données pour tests
</commit_message>
<xml_diff>
--- a/ProjetDocumentation/scenario_tests_spacelib.xlsx
+++ b/ProjetDocumentation/scenario_tests_spacelib.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\GitHub\ProjetSpacelib\ProjetDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>CAS</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>créer une nouvelle station avec -1 navette</t>
+  </si>
+  <si>
+    <t>ERREUR - réservation possible</t>
   </si>
 </sst>
 </file>
@@ -158,12 +161,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -258,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -269,6 +278,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,15 +562,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" customWidth="1"/>
     <col min="6" max="6" width="54" customWidth="1"/>
   </cols>
@@ -594,22 +605,26 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -624,7 +639,9 @@
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -639,7 +656,9 @@
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -654,7 +673,9 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
@@ -669,7 +690,9 @@
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -729,7 +752,9 @@
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">

</xml_diff>

<commit_message>
Scénario de test v1
Première version des scénarii de tests.
</commit_message>
<xml_diff>
--- a/ProjetDocumentation/scenario_tests_spacelib.xlsx
+++ b/ProjetDocumentation/scenario_tests_spacelib.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>CAS</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>ERREUR - réservation possible</t>
+  </si>
+  <si>
+    <t>A revérifier - crash appli - issue ouverte</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,22 +772,26 @@
       <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
@@ -799,7 +806,9 @@
       <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout de tests supplémentaires
</commit_message>
<xml_diff>
--- a/ProjetDocumentation/scenario_tests_spacelib.xlsx
+++ b/ProjetDocumentation/scenario_tests_spacelib.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="USER" sheetId="1" r:id="rId1"/>
+    <sheet name="ADMIN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
   <si>
     <t>CAS</t>
   </si>
@@ -56,9 +57,6 @@
     <t>1.2</t>
   </si>
   <si>
-    <t>réserver un nouvelle navette pour le même voyage</t>
-  </si>
-  <si>
     <t>Erreur - Une navette est déjà réservée</t>
   </si>
   <si>
@@ -86,68 +84,89 @@
     <t>choisir pour le voyage une navette qui est utilisée</t>
   </si>
   <si>
-    <t>choisir une station d'arrivée sans quai libre</t>
-  </si>
-  <si>
     <t>choisir une station de départ sans navette libre</t>
   </si>
   <si>
     <t>ADMIN</t>
   </si>
   <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>6.1</t>
-  </si>
-  <si>
     <t>créer une nouvelle station avec 0 navette</t>
   </si>
   <si>
-    <t>6.2</t>
-  </si>
-  <si>
     <t>créer une nouvelle station avec 1 navette</t>
   </si>
   <si>
-    <t>6.3</t>
-  </si>
-  <si>
     <t>créer une nouvelle station avec -1 navette</t>
   </si>
   <si>
-    <t>ERREUR - réservation possible</t>
-  </si>
-  <si>
-    <t>A revérifier - crash appli - issue ouverte</t>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>réserver une nouvelle navette pour le même voyage</t>
+  </si>
+  <si>
+    <t>choisir un jour où on a déjà un voyage prévu</t>
+  </si>
+  <si>
+    <t>créer une station avec une navette à 4 places</t>
+  </si>
+  <si>
+    <t>créer une station avec une navette à 2 places</t>
+  </si>
+  <si>
+    <t>créer une station avec une navette à 5 places</t>
+  </si>
+  <si>
+    <t>créer une station avec une navette à 10 places</t>
+  </si>
+  <si>
+    <t>créer une station avec une navette à 15 places</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>Test difficile</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>choisir une station de départ où il n'y a pas de quai libre</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>SELECT * FROM SPACELIBDB.NAVETTE WHERE ID = 76 FETCH FIRST 100 ROWS ONLY;</t>
+  </si>
+  <si>
+    <t>UPDATE SPACELIBDB.NAVETTE SET NBVOYAGES = 0 WHERE ID = 76;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST N1.7 - DONNEES : </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +182,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +202,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -266,16 +303,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -283,6 +332,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F15"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,235 +638,404 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
+      <c r="F3" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="E5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>16</v>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>16</v>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>13</v>
+      <c r="E9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nouveaux tests ajoutés (TNR)
</commit_message>
<xml_diff>
--- a/ProjetDocumentation/scenario_tests_spacelib.xlsx
+++ b/ProjetDocumentation/scenario_tests_spacelib.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
     <sheet name="ADMIN" sheetId="2" r:id="rId2"/>
+    <sheet name="MECA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="56">
   <si>
     <t>CAS</t>
   </si>
@@ -138,9 +139,6 @@
     <t>1.8</t>
   </si>
   <si>
-    <t>Test difficile</t>
-  </si>
-  <si>
     <t>1.9</t>
   </si>
   <si>
@@ -160,6 +158,42 @@
   </si>
   <si>
     <t xml:space="preserve">TEST N1.7 - DONNEES : </t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>MECA</t>
+  </si>
+  <si>
+    <t>réparer une navette</t>
+  </si>
+  <si>
+    <t>réparer une navette qui n'est pas à répar.</t>
+  </si>
+  <si>
+    <t>valider fin de révision</t>
+  </si>
+  <si>
+    <t>annuler un voyage planifié</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>annuler un voyage en cours</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>annuler un voyage ayant déjà eu lieu</t>
+  </si>
+  <si>
+    <t>réserver un voyage qui aura lieu dans le passé</t>
+  </si>
+  <si>
+    <t>Possible</t>
   </si>
 </sst>
 </file>
@@ -189,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,12 +242,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -224,26 +252,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -251,15 +259,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -318,30 +317,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,228 +672,290 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -873,7 +969,7 @@
   <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,155 +982,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="E7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1042,4 +1138,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>